<commit_message>
added time string parsing to int array and time format check
</commit_message>
<xml_diff>
--- a/brandNewSheet.xlsx
+++ b/brandNewSheet.xlsx
@@ -1,16 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
-  <sheets/>
+  <sheets>
+    <sheet name="Schedule Table" r:id="rId3" sheetId="1"/>
+  </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>This is Cell 1A</t>
+  </si>
+  <si>
+    <t>Let's put some effort into this program so people can actually use it!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45,8 +54,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="true"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A8"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added week day row inclusion during template creation. Also added provisional styles to sheet creation.
</commit_message>
<xml_diff>
--- a/brandNewSheet.xlsx
+++ b/brandNewSheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>6:00AM</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>10:00PM</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -127,15 +142,37 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -143,14 +180,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="bottom" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -158,184 +250,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A68"/>
+  <dimension ref="A1:U68"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1"/>
+      <c r="B1" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" t="s" s="3">
+        <v>36</v>
+      </c>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s">
+      <c r="A64" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s">
+      <c r="A66" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68"/>
+      <c r="A68" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added functionality to add classes to schedule, improved formatting
</commit_message>
<xml_diff>
--- a/brandNewSheet.xlsx
+++ b/brandNewSheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>6:00AM</t>
   </si>
@@ -126,6 +126,13 @@
   </si>
   <si>
     <t>Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello </t>
+  </si>
+  <si>
+    <t>this is kevin 
+ how are you</t>
   </si>
 </sst>
 </file>
@@ -302,6 +309,9 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">

</xml_diff>